<commit_message>
[FIX] project: avoid test failure due to duplicate stage names in demo data
Before this commit:
The test TestImportFiles was failing with demo data because multiple stages shared the same name on the test db.

After this commit:
The template now avoids relying on those demo data stages, which prevents the conflict and lets the test pass.

closes odoo/odoo#218821

Signed-off-by: Xavier Bol (xbo) <xbo@odoo.com>
</commit_message>
<xml_diff>
--- a/addons/project/static/xls/tasks_import_template.xlsx
+++ b/addons/project/static/xls/tasks_import_template.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="37">
   <si>
     <t>Title*</t>
   </si>
@@ -58,7 +58,7 @@
     <t>Home Construction</t>
   </si>
   <si>
-    <t>New</t>
+    <t>New (Home Construction)</t>
   </si>
   <si>
     <t>In Progress</t>
@@ -76,12 +76,15 @@
     <t>The customer requests a new meeting to launch the second phase of the project</t>
   </si>
   <si>
-    <t>Kitchen</t>
+    <t>Kitchen Renovations</t>
   </si>
   <si>
     <t>Renovations</t>
   </si>
   <si>
+    <t>In Progress (Renovations)</t>
+  </si>
+  <si>
     <t>Azure Interior, Brandon Freeman</t>
   </si>
   <si>
@@ -98,6 +101,9 @@
   </si>
   <si>
     <t>Furnitures</t>
+  </si>
+  <si>
+    <t>New (Renovations)</t>
   </si>
   <si>
     <t>Changes Requested</t>
@@ -128,7 +134,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -145,8 +151,20 @@
     </font>
     <font>
       <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Lato"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
-      <name val="Lato"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -188,23 +206,23 @@
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -569,7 +587,7 @@
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
@@ -610,13 +628,13 @@
         <v>21</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>15</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F3" s="5">
         <f>TODAY()-10</f>
@@ -627,34 +645,34 @@
         <v>25569.041666666668</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="L3" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
       <c r="A4" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="5">
@@ -662,16 +680,16 @@
         <v>25569.041666666668</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="L4" s="3" t="s">
         <v>20</v>
@@ -679,19 +697,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
       <c r="A5" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>15</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F5" s="7"/>
       <c r="G5" s="5">
@@ -699,13 +717,13 @@
         <v>25569.041666666668</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="K5" s="6"/>
       <c r="L5" s="3" t="s">
@@ -714,19 +732,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
       <c r="A6" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="5">
@@ -734,16 +752,16 @@
         <v>25569.041666666668</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="L6" s="3" t="s">
         <v>20</v>

</xml_diff>